<commit_message>
- Charts for documentation - fix: brightness off removes auto mode - diagnose p<nn>s
</commit_message>
<xml_diff>
--- a/doc/charts/RaumVerlassen.xlsx
+++ b/doc/charts/RaumVerlassen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D019748\PlatformIO\OpenKNX\OAM-PresenceModule\doc\charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B9265F-98AA-4D76-A6F2-70F248445FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E78964-179D-4B01-8FA1-0935DC897E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="4" xr2:uid="{7E41F7A6-C21A-4730-A43A-9C6130B28DC8}"/>
   </bookViews>
@@ -9033,16 +9033,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>16668</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4763</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>547687</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>166688</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>4763</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9074,16 +9074,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>16668</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>642938</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>547687</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>166688</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>4763</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9117,16 +9117,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>16668</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7144</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>547687</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>166688</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>23813</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>147638</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9160,16 +9160,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>16668</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>547687</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>166688</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>4764</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9203,16 +9203,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>16668</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>547687</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>166688</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>642937</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9542,7 +9542,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9961,7 +9961,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10380,7 +10380,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10798,8 +10798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A3F375-D835-4B1F-9E76-1FDDA130699B}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11263,8 +11263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498C5398-61C1-45A5-97B8-F6C257014C5F}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>